<commit_message>
WEEK 04-27 last edit
</commit_message>
<xml_diff>
--- a/WEEK formos/WEEK 04-27.xlsx
+++ b/WEEK formos/WEEK 04-27.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaponnik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaponnik\Desktop\git repos\TSP\WEEK formos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A5DCB9AD-87EC-4447-9C3B-E868A74717EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{13D53E20-822D-4633-8161-2782AB061324}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -915,8 +915,8 @@
   <sheetPr codeName="WeekSummary"/>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="5">
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
       <c r="G24" s="5">
         <f>C24</f>
@@ -1306,11 +1306,11 @@
         <v>5.5</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" ref="G25:G35" si="0">C25</f>
+        <f t="shared" ref="G25:G28" si="0">C25</f>
         <v>6.5</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" ref="I25:I35" si="1">C25</f>
+        <f t="shared" ref="I25:I28" si="1">C25</f>
         <v>6.5</v>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="4">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>

</xml_diff>